<commit_message>
Modified locations of outputs for screenshots and logging folders.
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/EmployeeContactData.xlsx
+++ b/src/test/resources/testData/EmployeeContactData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\magre\IdeaProjects\Group5B16\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC9C55E2-2547-46B1-9E40-341CF00C6E84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{750A346D-824F-43AA-A175-9FB04B4B6049}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Address Street 1</t>
   </si>
@@ -74,21 +74,6 @@
   </si>
   <si>
     <t>SC</t>
-  </si>
-  <si>
-    <t>987 Emory Dr</t>
-  </si>
-  <si>
-    <t>4567 Circle</t>
-  </si>
-  <si>
-    <t>Greenville</t>
-  </si>
-  <si>
-    <t>test@mail.gov</t>
-  </si>
-  <si>
-    <t>work@test.info</t>
   </si>
 </sst>
 </file>
@@ -431,7 +416,7 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -519,46 +504,13 @@
       </c>
     </row>
     <row r="3" spans="1:11">
-      <c r="A3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3">
-        <v>98765</v>
-      </c>
-      <c r="F3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3">
-        <v>123456789</v>
-      </c>
-      <c r="H3">
-        <v>9874561230</v>
-      </c>
-      <c r="I3">
-        <v>6541230789</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>22</v>
-      </c>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="J2" r:id="rId1" tooltip="mailto:catty@gmail.com" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="K2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="J3" r:id="rId3" xr:uid="{ACBD32FC-53D0-42C8-AD86-F7125BF4FCE6}"/>
-    <hyperlink ref="K3" r:id="rId4" xr:uid="{02E0265D-86D7-4649-8C20-62896F4798EF}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>